<commit_message>
Initial commit - add gitignore
</commit_message>
<xml_diff>
--- a/documents/Traveler Researcher.xlsx
+++ b/documents/Traveler Researcher.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Carleton\Assignments\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Carleton\Assignments\Projects\Project-01\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EA43694-784C-4A22-8541-3FF82802DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FEFEF8-4396-4FE7-9CE0-8B3C17E440A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{249E9CF8-86E5-4F6D-857C-31117DDEB3C4}"/>
   </bookViews>
@@ -319,6 +319,26 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,45 +360,25 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="9" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -427,7 +427,7 @@
         <xdr:cNvPr id="3" name="Graphic 2" descr="Hummingbird">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E77598F-AE72-7DC7-A53D-354BEF2A3E96}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -480,7 +480,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4895F33D-E61B-CC43-2F61-20E8F0A0DB4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -559,7 +559,7 @@
         <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442FF04E-F1DA-57C2-5C46-AC987A810BDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -619,7 +619,7 @@
         <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906C63A4-ED3A-34B9-2AF0-E62C91E237EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -695,7 +695,7 @@
         <xdr:cNvPr id="9" name="Rectangle: Rounded Corners 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FD146B0-BFB6-8DD0-DBE7-4A8FAAB9B341}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -758,7 +758,7 @@
         <xdr:cNvPr id="33" name="Group 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268110A1-0868-5442-0D11-AB9EB0C6D919}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -777,7 +777,7 @@
           <xdr:cNvPr id="14" name="Group 13">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49F9B761-44AB-68C2-DE67-1BC6322F328C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -796,7 +796,7 @@
             <xdr:cNvPr id="10" name="Rectangle 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ACAFC3A-E63B-8FA5-4210-328556DE6F94}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -841,7 +841,7 @@
             <xdr:cNvPr id="11" name="TextBox 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD53A003-C309-C4DC-DF56-F2A014D70325}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -920,7 +920,7 @@
             <xdr:cNvPr id="13" name="Picture 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF33DE09-78D8-EBBB-7909-3AF7ADAB428A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -971,7 +971,7 @@
           <xdr:cNvPr id="15" name="Group 14">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB0FB1B-C58E-4AC8-9E9B-86D8726E92C0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -990,7 +990,7 @@
             <xdr:cNvPr id="16" name="Rectangle 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391D9958-9C22-3E82-F879-3F22D8362C80}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1035,7 +1035,7 @@
             <xdr:cNvPr id="17" name="TextBox 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B638AB3E-778E-B619-75BA-1AD2A98256DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1114,7 +1114,7 @@
             <xdr:cNvPr id="18" name="Picture 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE76BE3B-B3E1-D1D3-0545-E6AF718D6DEB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1165,7 +1165,7 @@
           <xdr:cNvPr id="19" name="Group 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14329A99-20DA-41DA-9D98-02951BC29E24}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1184,7 +1184,7 @@
             <xdr:cNvPr id="20" name="Rectangle 19">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F983FE39-F3B9-45BE-2413-9EE1DDCAABB6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1229,7 +1229,7 @@
             <xdr:cNvPr id="21" name="TextBox 20">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1FF41EF-4E40-C7B0-1F09-11D1669864CE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1308,7 +1308,7 @@
             <xdr:cNvPr id="22" name="Picture 21">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{613F1059-02F6-1BD4-EA0F-9C1A40D5E936}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
           <xdr:cNvPr id="23" name="Group 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{375DC9ED-E6EE-4711-B2C7-33E73FF6CCCB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1378,7 +1378,7 @@
             <xdr:cNvPr id="24" name="Rectangle 23">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71C1BE7C-90A3-004E-413A-85DEFE2319B6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1423,7 +1423,7 @@
             <xdr:cNvPr id="25" name="TextBox 24">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAD5343E-A55D-C71B-F51B-AD920C2251EE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1502,7 +1502,7 @@
             <xdr:cNvPr id="26" name="Picture 25">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4585746E-3335-AC02-5E19-E791DB7FE6B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1569,7 +1569,7 @@
         <xdr:cNvPr id="27" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6369B53-027F-3AD2-FCD9-C92496CE5AC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1639,7 +1639,7 @@
         <xdr:cNvPr id="28" name="TextBox 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F17ADCE-AF81-E57D-F823-AF60B2A1FA5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,7 +1713,7 @@
         <xdr:cNvPr id="29" name="Oval 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01054AE1-7F1F-3F58-6F9B-7776381E3E51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1773,7 +1773,7 @@
         <xdr:cNvPr id="30" name="Oval 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{155727DE-FFB0-B96D-8FDA-AF97841D0BBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1833,7 +1833,7 @@
         <xdr:cNvPr id="31" name="TextBox 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D718EEE8-48F0-0317-7C67-7776EB47160B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1907,7 +1907,7 @@
         <xdr:cNvPr id="32" name="TextBox 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBC5F2A2-BE04-0BC5-86D4-E5E4E78D751D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,7 +1981,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB3FAA75-37BE-1A99-FFC3-77DEDCA01D58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2051,7 +2051,7 @@
         <xdr:cNvPr id="35" name="TextBox 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79746540-03C6-2B94-6F1A-CA015B015FD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2130,7 +2130,7 @@
         <xdr:cNvPr id="2" name="Graphic 1" descr="Hummingbird">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C508DF-FCAD-4F84-A445-33D64B7FC58C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2183,7 +2183,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9239AEF6-194E-47E3-9194-DACD1C6889CD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2267,7 +2267,7 @@
         <xdr:cNvPr id="2" name="Graphic 1" descr="Hummingbird">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5246B11A-9B5E-4392-A5B2-831CD4CE3DC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2320,7 +2320,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13318C59-9252-4C35-95BA-EACC36175F82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2751,695 +2751,695 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="4"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="7"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="7"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="7"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="9"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
-      <c r="K53" s="10"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3477,569 +3477,569 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="13" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="13" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="13" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="17"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="20" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="8"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="21">
+      <c r="A11" s="1"/>
+      <c r="B11" s="9">
         <v>45184</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="21">
+      <c r="C11" s="1"/>
+      <c r="D11" s="9">
         <v>45184</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="22">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="10">
         <v>1205</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="21">
+      <c r="A12" s="1"/>
+      <c r="B12" s="9">
         <v>45184</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="21">
+      <c r="C12" s="1"/>
+      <c r="D12" s="9">
         <v>45184</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="22">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="10">
         <v>1206</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="13">
         <v>45184</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27">
+      <c r="C13" s="14"/>
+      <c r="D13" s="15">
         <v>45184</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16">
         <v>1207</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="29" t="s">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="8"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="21">
+      <c r="A14" s="1"/>
+      <c r="B14" s="9">
         <v>45184</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="21">
+      <c r="C14" s="1"/>
+      <c r="D14" s="9">
         <v>45184</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="22">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="10">
         <v>1208</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="21">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9">
         <v>45184</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="21">
+      <c r="C15" s="1"/>
+      <c r="D15" s="9">
         <v>45184</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="22">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="10">
         <v>1209</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="21">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9">
         <v>45184</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="21">
+      <c r="C16" s="1"/>
+      <c r="D16" s="9">
         <v>45184</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="22">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="10">
         <v>1210</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="21">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9">
         <v>45184</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="21">
+      <c r="C17" s="1"/>
+      <c r="D17" s="9">
         <v>45184</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="22">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="10">
         <v>1211</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="21">
+      <c r="A18" s="1"/>
+      <c r="B18" s="9">
         <v>45184</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="21">
+      <c r="C18" s="1"/>
+      <c r="D18" s="9">
         <v>45184</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="22">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="10">
         <v>1212</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="21">
+      <c r="A19" s="1"/>
+      <c r="B19" s="9">
         <v>45184</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="21">
+      <c r="C19" s="1"/>
+      <c r="D19" s="9">
         <v>45184</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="22">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="10">
         <v>1213</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="21">
+      <c r="A20" s="1"/>
+      <c r="B20" s="9">
         <v>45184</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="21">
+      <c r="C20" s="1"/>
+      <c r="D20" s="9">
         <v>45184</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="22">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="10">
         <v>1214</v>
       </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="21">
+      <c r="A21" s="1"/>
+      <c r="B21" s="9">
         <v>45184</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="21">
+      <c r="C21" s="1"/>
+      <c r="D21" s="9">
         <v>45184</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="22">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="10">
         <v>1215</v>
       </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="21">
+      <c r="A22" s="1"/>
+      <c r="B22" s="9">
         <v>45184</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="21">
+      <c r="C22" s="1"/>
+      <c r="D22" s="9">
         <v>45184</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="22">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="10">
         <v>1216</v>
       </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="21">
+      <c r="A23" s="1"/>
+      <c r="B23" s="9">
         <v>45184</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="21">
+      <c r="C23" s="1"/>
+      <c r="D23" s="9">
         <v>45184</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="22">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="10">
         <v>1217</v>
       </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4066,7 +4066,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A1:M31"/>
+      <selection activeCell="D4" sqref="D4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,541 +4082,541 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="20" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="8"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="21">
+      <c r="A11" s="1"/>
+      <c r="B11" s="9">
         <v>45184</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="21" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="22" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="22">
+      <c r="H11" s="1"/>
+      <c r="I11" s="10">
         <v>1205</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="21">
+      <c r="A12" s="1"/>
+      <c r="B12" s="9">
         <v>45184</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="22" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="22">
+      <c r="H12" s="1"/>
+      <c r="I12" s="10">
         <v>1206</v>
       </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="13">
         <v>45184</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="28">
+      <c r="H13" s="14"/>
+      <c r="I13" s="16">
         <v>1207</v>
       </c>
-      <c r="J13" s="26"/>
-      <c r="K13" s="29" t="s">
+      <c r="J13" s="14"/>
+      <c r="K13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="8"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="21">
+      <c r="A14" s="1"/>
+      <c r="B14" s="9">
         <v>45184</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="22" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="22">
+      <c r="H14" s="1"/>
+      <c r="I14" s="10">
         <v>1208</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="21">
+      <c r="A15" s="1"/>
+      <c r="B15" s="9">
         <v>45184</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="21" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="22" t="s">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="22">
+      <c r="H15" s="1"/>
+      <c r="I15" s="10">
         <v>1209</v>
       </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="21">
+      <c r="A16" s="1"/>
+      <c r="B16" s="9">
         <v>45184</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="22" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="22">
+      <c r="H16" s="1"/>
+      <c r="I16" s="10">
         <v>1210</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="21">
+      <c r="A17" s="1"/>
+      <c r="B17" s="9">
         <v>45184</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="22" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="22">
+      <c r="H17" s="1"/>
+      <c r="I17" s="10">
         <v>1211</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Initial commit - add API parameters
</commit_message>
<xml_diff>
--- a/documents/Traveler Researcher.xlsx
+++ b/documents/Traveler Researcher.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Carleton\Assignments\Projects\Project-01\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FEFEF8-4396-4FE7-9CE0-8B3C17E440A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1019D549-DBF4-4821-BFBC-176CA793B052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{249E9CF8-86E5-4F6D-857C-31117DDEB3C4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{249E9CF8-86E5-4F6D-857C-31117DDEB3C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Index.html" sheetId="1" r:id="rId1"/>
     <sheet name="Search.html" sheetId="2" r:id="rId2"/>
     <sheet name="History.html" sheetId="4" r:id="rId3"/>
+    <sheet name="Popup" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Carleton Unversity - Coding boot camp v2023.001</t>
   </si>
@@ -85,6 +86,12 @@
   <si>
     <t>WestJet</t>
   </si>
+  <si>
+    <t>Error has ocurred!</t>
+  </si>
+  <si>
+    <t>Some message or form</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +152,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +217,17 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -309,15 +341,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -381,9 +415,20 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="40% - Accent3" xfId="5" builtinId="39"/>
+    <cellStyle name="40% - Accent5" xfId="7" builtinId="47"/>
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -2387,13 +2432,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>2</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>561975</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2439,6 +2484,74 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB617DA0-8482-33E7-4E3B-2DE5353C2F70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1409700" y="1781175"/>
+          <a:ext cx="1476375" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>Close</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4063,10 +4176,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:K4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4111,39 +4224,39 @@
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
     </row>
-    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -4159,11 +4272,11 @@
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="30"/>
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -4192,18 +4305,20 @@
     </row>
     <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="B8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -4220,47 +4335,31 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="9">
-        <v>45184</v>
-      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="10">
-        <v>1205</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -4268,50 +4367,48 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="9">
-        <v>45184</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="10">
-        <v>1206</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="13">
+      <c r="B13" s="9">
         <v>45184</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="16">
-        <v>1207</v>
-      </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13" s="27"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="10">
+        <v>1205</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -4321,7 +4418,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4330,7 +4427,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="10">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -4339,25 +4436,27 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="9">
+      <c r="B15" s="13">
         <v>45184</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="10">
-        <v>1209</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="16">
+        <v>1207</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="27"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -4367,7 +4466,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -4376,7 +4475,7 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="10">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -4390,16 +4489,16 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="10">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -4408,14 +4507,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="9">
+        <v>45184</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="I18" s="10">
+        <v>1210</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -4423,14 +4530,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="9">
+        <v>45184</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="10">
+        <v>1211</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -4455,10 +4570,10 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="10"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -4470,10 +4585,10 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="9"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -4602,28 +4717,59 @@
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="A31:M31"/>
+  <mergeCells count="5">
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="A33:M33"/>
     <mergeCell ref="A1:M2"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A3:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="83" orientation="portrait" r:id="rId1"/>
@@ -4638,13 +4784,13 @@
               <from>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
+                <xdr:row>4</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
                 <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
@@ -4657,4 +4803,134 @@
     </mc:AlternateContent>
   </controls>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CA5FCC-BAF3-4D9E-85A5-DCF44445605E}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>